<commit_message>
Remove highlighting from parts that have arrived
</commit_message>
<xml_diff>
--- a/r2/build/tr20-r2-bom/tr20-r2.xlsx
+++ b/r2/build/tr20-r2-bom/tr20-r2.xlsx
@@ -1136,11 +1136,12 @@
     <numFmt numFmtId="169" formatCode="0.00%"/>
     <numFmt numFmtId="170" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1162,6 +1163,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1169,12 +1171,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1182,6 +1186,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1189,24 +1194,28 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1214,6 +1223,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1221,24 +1231,36 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1480,11 +1502,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1492,7 +1514,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1500,11 +1522,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1616,13 +1638,13 @@
   </sheetPr>
   <dimension ref="A1:BL99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
@@ -4854,78 +4876,26 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B45" s="16" t="n">
+      <c r="B45" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="16"/>
-      <c r="S45" s="1" t="s">
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
+      <c r="O45" s="0"/>
+      <c r="P45" s="0"/>
+      <c r="S45" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="T45" s="17"/>
-      <c r="U45" s="16"/>
-      <c r="V45" s="17"/>
-      <c r="W45" s="16"/>
-      <c r="X45" s="16"/>
-      <c r="Y45" s="16"/>
-      <c r="Z45" s="16"/>
-      <c r="AA45" s="16"/>
-      <c r="AB45" s="16"/>
-      <c r="AC45" s="16"/>
-      <c r="AD45" s="16"/>
-      <c r="AE45" s="16"/>
-      <c r="AF45" s="16"/>
-      <c r="AG45" s="16"/>
-      <c r="AH45" s="16"/>
-      <c r="AI45" s="16"/>
-      <c r="AJ45" s="16"/>
-      <c r="AK45" s="16"/>
-      <c r="AL45" s="16"/>
-      <c r="AM45" s="16"/>
-      <c r="AN45" s="16"/>
-      <c r="AO45" s="16"/>
-      <c r="AP45" s="16"/>
-      <c r="AQ45" s="16"/>
-      <c r="AR45" s="16"/>
-      <c r="AS45" s="16"/>
-      <c r="AT45" s="16"/>
-      <c r="AU45" s="16"/>
-      <c r="AV45" s="16"/>
-      <c r="AW45" s="16"/>
-      <c r="AX45" s="16"/>
-      <c r="AY45" s="16"/>
-      <c r="AZ45" s="16"/>
-      <c r="BA45" s="16"/>
-      <c r="BB45" s="16"/>
-      <c r="BC45" s="16"/>
-      <c r="BD45" s="16"/>
-      <c r="BE45" s="16"/>
-      <c r="BF45" s="16"/>
-      <c r="BG45" s="16"/>
-      <c r="BH45" s="16"/>
-      <c r="BI45" s="16"/>
-      <c r="BJ45" s="16"/>
-      <c r="BK45" s="16"/>
-      <c r="BL45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -4966,7 +4936,7 @@
         <f aca="false">O46*$L$77</f>
         <v>3.864</v>
       </c>
-      <c r="R46" s="21" t="s">
+      <c r="R46" s="16" t="s">
         <v>225</v>
       </c>
       <c r="S46" s="1" t="s">
@@ -5474,108 +5444,61 @@
       <c r="S54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B55" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="15" t="s">
+      <c r="B55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="G55" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="H55" s="17"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18" t="str">
+      <c r="I55" s="0"/>
+      <c r="J55" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B55*$Q$80/I55,0), "" )</f>
         <v/>
       </c>
-      <c r="K55" s="18" t="n">
+      <c r="K55" s="0" t="n">
         <f aca="false">IF(I55&gt;0,I55*J55,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L55" s="19" t="n">
+      <c r="L55" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M55" s="20" t="n">
+      <c r="M55" s="0" t="n">
         <f aca="false">L55*$L$77</f>
         <v>0</v>
       </c>
-      <c r="N55" s="20" t="n">
+      <c r="N55" s="0" t="n">
         <f aca="false">8*L77</f>
         <v>1.12</v>
       </c>
-      <c r="O55" s="20" t="n">
+      <c r="O55" s="0" t="n">
         <f aca="false">K55*L55</f>
         <v>0</v>
       </c>
-      <c r="P55" s="18" t="n">
+      <c r="P55" s="0" t="n">
         <f aca="false">O55*$L$77</f>
         <v>0</v>
       </c>
-      <c r="Q55" s="17" t="s">
+      <c r="Q55" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="R55" s="17" t="s">
+      <c r="R55" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="S55" s="15" t="s">
+      <c r="S55" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="T55" s="17"/>
-      <c r="U55" s="16"/>
-      <c r="V55" s="17"/>
-      <c r="W55" s="16"/>
-      <c r="X55" s="16"/>
-      <c r="Y55" s="16"/>
-      <c r="Z55" s="16"/>
-      <c r="AA55" s="16"/>
-      <c r="AB55" s="16"/>
-      <c r="AC55" s="16"/>
-      <c r="AD55" s="16"/>
-      <c r="AE55" s="16"/>
-      <c r="AF55" s="16"/>
-      <c r="AG55" s="16"/>
-      <c r="AH55" s="16"/>
-      <c r="AI55" s="16"/>
-      <c r="AJ55" s="16"/>
-      <c r="AK55" s="16"/>
-      <c r="AL55" s="16"/>
-      <c r="AM55" s="16"/>
-      <c r="AN55" s="16"/>
-      <c r="AO55" s="16"/>
-      <c r="AP55" s="16"/>
-      <c r="AQ55" s="16"/>
-      <c r="AR55" s="16"/>
-      <c r="AS55" s="16"/>
-      <c r="AT55" s="16"/>
-      <c r="AU55" s="16"/>
-      <c r="AV55" s="16"/>
-      <c r="AW55" s="16"/>
-      <c r="AX55" s="16"/>
-      <c r="AY55" s="16"/>
-      <c r="AZ55" s="16"/>
-      <c r="BA55" s="16"/>
-      <c r="BB55" s="16"/>
-      <c r="BC55" s="16"/>
-      <c r="BD55" s="16"/>
-      <c r="BE55" s="16"/>
-      <c r="BF55" s="16"/>
-      <c r="BG55" s="16"/>
-      <c r="BH55" s="16"/>
-      <c r="BI55" s="16"/>
-      <c r="BJ55" s="16"/>
-      <c r="BK55" s="16"/>
-      <c r="BL55" s="16"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -5584,7 +5507,7 @@
       <c r="B56" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="0" t="s">
         <v>292</v>
       </c>
       <c r="E56" s="0" t="s">
@@ -5599,29 +5522,30 @@
       <c r="H56" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="J56" s="2" t="str">
+      <c r="I56" s="0"/>
+      <c r="J56" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B56*$Q$80/I56,0), "" )</f>
         <v/>
       </c>
-      <c r="K56" s="2" t="n">
+      <c r="K56" s="0" t="n">
         <f aca="false">IF(I56&gt;0,I56*J56,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L56" s="3" t="n">
+      <c r="L56" s="0" t="n">
         <v>3.22</v>
       </c>
-      <c r="M56" s="4" t="n">
+      <c r="M56" s="0" t="n">
         <f aca="false">L56*$L$77</f>
         <v>0.4508</v>
       </c>
-      <c r="N56" s="4" t="n">
+      <c r="N56" s="0" t="n">
         <v>0.34</v>
       </c>
-      <c r="O56" s="4" t="n">
+      <c r="O56" s="0" t="n">
         <f aca="false">K56*L56</f>
         <v>1771</v>
       </c>
-      <c r="P56" s="2" t="n">
+      <c r="P56" s="0" t="n">
         <f aca="false">O56*$L$77</f>
         <v>247.94</v>
       </c>
@@ -5631,93 +5555,43 @@
       <c r="R56" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="S56" s="1" t="s">
+      <c r="S56" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="T56" s="11"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="B57" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" s="16" t="s">
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18" t="n">
+      <c r="I57" s="0"/>
+      <c r="J57" s="0"/>
+      <c r="K57" s="0" t="n">
         <f aca="false">IF(I57&gt;0,I57*J57,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L57" s="19"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="17"/>
-      <c r="R57" s="17" t="s">
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="N57" s="0"/>
+      <c r="O57" s="0"/>
+      <c r="P57" s="0"/>
+      <c r="R57" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="S57" s="16" t="s">
+      <c r="S57" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="T57" s="16"/>
-      <c r="U57" s="16"/>
-      <c r="V57" s="17"/>
-      <c r="W57" s="16"/>
-      <c r="X57" s="16"/>
-      <c r="Y57" s="16"/>
-      <c r="Z57" s="16"/>
-      <c r="AA57" s="16"/>
-      <c r="AB57" s="16"/>
-      <c r="AC57" s="16"/>
-      <c r="AD57" s="16"/>
-      <c r="AE57" s="16"/>
-      <c r="AF57" s="16"/>
-      <c r="AG57" s="16"/>
-      <c r="AH57" s="16"/>
-      <c r="AI57" s="16"/>
-      <c r="AJ57" s="16"/>
-      <c r="AK57" s="16"/>
-      <c r="AL57" s="16"/>
-      <c r="AM57" s="16"/>
-      <c r="AN57" s="16"/>
-      <c r="AO57" s="16"/>
-      <c r="AP57" s="16"/>
-      <c r="AQ57" s="16"/>
-      <c r="AR57" s="16"/>
-      <c r="AS57" s="16"/>
-      <c r="AT57" s="16"/>
-      <c r="AU57" s="16"/>
-      <c r="AV57" s="16"/>
-      <c r="AW57" s="16"/>
-      <c r="AX57" s="16"/>
-      <c r="AY57" s="16"/>
-      <c r="AZ57" s="16"/>
-      <c r="BA57" s="16"/>
-      <c r="BB57" s="16"/>
-      <c r="BC57" s="16"/>
-      <c r="BD57" s="16"/>
-      <c r="BE57" s="16"/>
-      <c r="BF57" s="16"/>
-      <c r="BG57" s="16"/>
-      <c r="BH57" s="16"/>
-      <c r="BI57" s="16"/>
-      <c r="BJ57" s="16"/>
-      <c r="BK57" s="16"/>
-      <c r="BL57" s="16"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
@@ -6026,26 +5900,26 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="B64" s="16" t="n">
+      <c r="B64" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="F64" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="G64" s="16" t="s">
+      <c r="G64" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="H64" s="16"/>
+      <c r="H64" s="17"/>
       <c r="I64" s="18"/>
-      <c r="J64" s="22" t="str">
+      <c r="J64" s="19" t="str">
         <f aca="false">IFERROR( ROUNDUP(B64*$Q$80/I64,0), "" )</f>
         <v/>
       </c>
@@ -6053,7 +5927,7 @@
         <f aca="false">IF(I64&gt;0,I64*J64,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L64" s="16" t="n">
+      <c r="L64" s="17" t="n">
         <v>0</v>
       </c>
       <c r="M64" s="20" t="n">
@@ -6071,76 +5945,76 @@
         <f aca="false">O64*$L$77</f>
         <v>0</v>
       </c>
-      <c r="Q64" s="16" t="s">
+      <c r="Q64" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="R64" s="16" t="s">
+      <c r="R64" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="S64" s="16"/>
-      <c r="T64" s="16"/>
-      <c r="U64" s="16"/>
-      <c r="V64" s="16"/>
-      <c r="W64" s="16"/>
-      <c r="X64" s="16"/>
-      <c r="Y64" s="16"/>
-      <c r="Z64" s="16"/>
-      <c r="AA64" s="16"/>
-      <c r="AB64" s="16"/>
-      <c r="AC64" s="16"/>
-      <c r="AD64" s="16"/>
-      <c r="AE64" s="16"/>
-      <c r="AF64" s="16"/>
-      <c r="AG64" s="16"/>
-      <c r="AH64" s="16"/>
-      <c r="AI64" s="16"/>
-      <c r="AJ64" s="16"/>
-      <c r="AK64" s="16"/>
-      <c r="AL64" s="16"/>
-      <c r="AM64" s="16"/>
-      <c r="AN64" s="16"/>
-      <c r="AO64" s="16"/>
-      <c r="AP64" s="16"/>
-      <c r="AQ64" s="16"/>
-      <c r="AR64" s="16"/>
-      <c r="AS64" s="16"/>
-      <c r="AT64" s="16"/>
-      <c r="AU64" s="16"/>
-      <c r="AV64" s="16"/>
-      <c r="AW64" s="16"/>
-      <c r="AX64" s="16"/>
-      <c r="AY64" s="16"/>
-      <c r="AZ64" s="16"/>
-      <c r="BA64" s="16"/>
-      <c r="BB64" s="16"/>
-      <c r="BC64" s="16"/>
-      <c r="BD64" s="16"/>
-      <c r="BE64" s="16"/>
-      <c r="BF64" s="16"/>
-      <c r="BG64" s="16"/>
-      <c r="BH64" s="16"/>
-      <c r="BI64" s="16"/>
-      <c r="BJ64" s="16"/>
-      <c r="BK64" s="16"/>
-      <c r="BL64" s="16"/>
+      <c r="S64" s="17"/>
+      <c r="T64" s="17"/>
+      <c r="U64" s="17"/>
+      <c r="V64" s="17"/>
+      <c r="W64" s="17"/>
+      <c r="X64" s="17"/>
+      <c r="Y64" s="17"/>
+      <c r="Z64" s="17"/>
+      <c r="AA64" s="17"/>
+      <c r="AB64" s="17"/>
+      <c r="AC64" s="17"/>
+      <c r="AD64" s="17"/>
+      <c r="AE64" s="17"/>
+      <c r="AF64" s="17"/>
+      <c r="AG64" s="17"/>
+      <c r="AH64" s="17"/>
+      <c r="AI64" s="17"/>
+      <c r="AJ64" s="17"/>
+      <c r="AK64" s="17"/>
+      <c r="AL64" s="17"/>
+      <c r="AM64" s="17"/>
+      <c r="AN64" s="17"/>
+      <c r="AO64" s="17"/>
+      <c r="AP64" s="17"/>
+      <c r="AQ64" s="17"/>
+      <c r="AR64" s="17"/>
+      <c r="AS64" s="17"/>
+      <c r="AT64" s="17"/>
+      <c r="AU64" s="17"/>
+      <c r="AV64" s="17"/>
+      <c r="AW64" s="17"/>
+      <c r="AX64" s="17"/>
+      <c r="AY64" s="17"/>
+      <c r="AZ64" s="17"/>
+      <c r="BA64" s="17"/>
+      <c r="BB64" s="17"/>
+      <c r="BC64" s="17"/>
+      <c r="BD64" s="17"/>
+      <c r="BE64" s="17"/>
+      <c r="BF64" s="17"/>
+      <c r="BG64" s="17"/>
+      <c r="BH64" s="17"/>
+      <c r="BI64" s="17"/>
+      <c r="BJ64" s="17"/>
+      <c r="BK64" s="17"/>
+      <c r="BL64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="B65" s="16" t="n">
+      <c r="B65" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
       <c r="I65" s="18"/>
-      <c r="J65" s="16" t="str">
+      <c r="J65" s="17" t="str">
         <f aca="false">IFERROR( ROUNDUP(B65*$Q$80/I65,0), "" )</f>
         <v/>
       </c>
@@ -6148,7 +6022,7 @@
         <f aca="false">IF(I65&gt;0,I65*J65,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L65" s="19"/>
+      <c r="L65" s="21"/>
       <c r="M65" s="20" t="n">
         <f aca="false">L65*$L$77</f>
         <v>0</v>
@@ -6164,74 +6038,74 @@
         <f aca="false">O65*$L$77</f>
         <v>0</v>
       </c>
-      <c r="Q65" s="16"/>
-      <c r="R65" s="16"/>
-      <c r="S65" s="16"/>
-      <c r="T65" s="16"/>
-      <c r="U65" s="16"/>
-      <c r="V65" s="16"/>
-      <c r="W65" s="16"/>
-      <c r="X65" s="16"/>
-      <c r="Y65" s="16"/>
-      <c r="Z65" s="16"/>
-      <c r="AA65" s="16"/>
-      <c r="AB65" s="16"/>
-      <c r="AC65" s="16"/>
-      <c r="AD65" s="16"/>
-      <c r="AE65" s="16"/>
-      <c r="AF65" s="16"/>
-      <c r="AG65" s="16"/>
-      <c r="AH65" s="16"/>
-      <c r="AI65" s="16"/>
-      <c r="AJ65" s="16"/>
-      <c r="AK65" s="16"/>
-      <c r="AL65" s="16"/>
-      <c r="AM65" s="16"/>
-      <c r="AN65" s="16"/>
-      <c r="AO65" s="16"/>
-      <c r="AP65" s="16"/>
-      <c r="AQ65" s="16"/>
-      <c r="AR65" s="16"/>
-      <c r="AS65" s="16"/>
-      <c r="AT65" s="16"/>
-      <c r="AU65" s="16"/>
-      <c r="AV65" s="16"/>
-      <c r="AW65" s="16"/>
-      <c r="AX65" s="16"/>
-      <c r="AY65" s="16"/>
-      <c r="AZ65" s="16"/>
-      <c r="BA65" s="16"/>
-      <c r="BB65" s="16"/>
-      <c r="BC65" s="16"/>
-      <c r="BD65" s="16"/>
-      <c r="BE65" s="16"/>
-      <c r="BF65" s="16"/>
-      <c r="BG65" s="16"/>
-      <c r="BH65" s="16"/>
-      <c r="BI65" s="16"/>
-      <c r="BJ65" s="16"/>
-      <c r="BK65" s="16"/>
-      <c r="BL65" s="16"/>
+      <c r="Q65" s="17"/>
+      <c r="R65" s="17"/>
+      <c r="S65" s="17"/>
+      <c r="T65" s="17"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="17"/>
+      <c r="W65" s="17"/>
+      <c r="X65" s="17"/>
+      <c r="Y65" s="17"/>
+      <c r="Z65" s="17"/>
+      <c r="AA65" s="17"/>
+      <c r="AB65" s="17"/>
+      <c r="AC65" s="17"/>
+      <c r="AD65" s="17"/>
+      <c r="AE65" s="17"/>
+      <c r="AF65" s="17"/>
+      <c r="AG65" s="17"/>
+      <c r="AH65" s="17"/>
+      <c r="AI65" s="17"/>
+      <c r="AJ65" s="17"/>
+      <c r="AK65" s="17"/>
+      <c r="AL65" s="17"/>
+      <c r="AM65" s="17"/>
+      <c r="AN65" s="17"/>
+      <c r="AO65" s="17"/>
+      <c r="AP65" s="17"/>
+      <c r="AQ65" s="17"/>
+      <c r="AR65" s="17"/>
+      <c r="AS65" s="17"/>
+      <c r="AT65" s="17"/>
+      <c r="AU65" s="17"/>
+      <c r="AV65" s="17"/>
+      <c r="AW65" s="17"/>
+      <c r="AX65" s="17"/>
+      <c r="AY65" s="17"/>
+      <c r="AZ65" s="17"/>
+      <c r="BA65" s="17"/>
+      <c r="BB65" s="17"/>
+      <c r="BC65" s="17"/>
+      <c r="BD65" s="17"/>
+      <c r="BE65" s="17"/>
+      <c r="BF65" s="17"/>
+      <c r="BG65" s="17"/>
+      <c r="BH65" s="17"/>
+      <c r="BI65" s="17"/>
+      <c r="BJ65" s="17"/>
+      <c r="BK65" s="17"/>
+      <c r="BL65" s="17"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="B66" s="16" t="n">
+      <c r="B66" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16" t="s">
+      <c r="D66" s="17"/>
+      <c r="E66" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
       <c r="I66" s="18"/>
-      <c r="J66" s="16" t="str">
+      <c r="J66" s="17" t="str">
         <f aca="false">IFERROR( ROUNDUP(B66*$Q$80/I66,0), "" )</f>
         <v/>
       </c>
@@ -6239,7 +6113,7 @@
         <f aca="false">IF(I66&gt;0,I66*J66,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L66" s="19"/>
+      <c r="L66" s="21"/>
       <c r="M66" s="20" t="n">
         <f aca="false">L66*$L$77</f>
         <v>0</v>
@@ -6255,74 +6129,74 @@
         <f aca="false">O66*$L$77</f>
         <v>0</v>
       </c>
-      <c r="Q66" s="16"/>
-      <c r="R66" s="16" t="s">
+      <c r="Q66" s="17"/>
+      <c r="R66" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="S66" s="16"/>
-      <c r="T66" s="16" t="s">
+      <c r="S66" s="17"/>
+      <c r="T66" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="U66" s="16"/>
-      <c r="V66" s="16"/>
-      <c r="W66" s="16"/>
-      <c r="X66" s="16"/>
-      <c r="Y66" s="16"/>
-      <c r="Z66" s="16"/>
-      <c r="AA66" s="16"/>
-      <c r="AB66" s="16"/>
-      <c r="AC66" s="16"/>
-      <c r="AD66" s="16"/>
-      <c r="AE66" s="16"/>
-      <c r="AF66" s="16"/>
-      <c r="AG66" s="16"/>
-      <c r="AH66" s="16"/>
-      <c r="AI66" s="16"/>
-      <c r="AJ66" s="16"/>
-      <c r="AK66" s="16"/>
-      <c r="AL66" s="16"/>
-      <c r="AM66" s="16"/>
-      <c r="AN66" s="16"/>
-      <c r="AO66" s="16"/>
-      <c r="AP66" s="16"/>
-      <c r="AQ66" s="16"/>
-      <c r="AR66" s="16"/>
-      <c r="AS66" s="16"/>
-      <c r="AT66" s="16"/>
-      <c r="AU66" s="16"/>
-      <c r="AV66" s="16"/>
-      <c r="AW66" s="16"/>
-      <c r="AX66" s="16"/>
-      <c r="AY66" s="16"/>
-      <c r="AZ66" s="16"/>
-      <c r="BA66" s="16"/>
-      <c r="BB66" s="16"/>
-      <c r="BC66" s="16"/>
-      <c r="BD66" s="16"/>
-      <c r="BE66" s="16"/>
-      <c r="BF66" s="16"/>
-      <c r="BG66" s="16"/>
-      <c r="BH66" s="16"/>
-      <c r="BI66" s="16"/>
-      <c r="BJ66" s="16"/>
-      <c r="BK66" s="16"/>
-      <c r="BL66" s="16"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="17"/>
+      <c r="X66" s="17"/>
+      <c r="Y66" s="17"/>
+      <c r="Z66" s="17"/>
+      <c r="AA66" s="17"/>
+      <c r="AB66" s="17"/>
+      <c r="AC66" s="17"/>
+      <c r="AD66" s="17"/>
+      <c r="AE66" s="17"/>
+      <c r="AF66" s="17"/>
+      <c r="AG66" s="17"/>
+      <c r="AH66" s="17"/>
+      <c r="AI66" s="17"/>
+      <c r="AJ66" s="17"/>
+      <c r="AK66" s="17"/>
+      <c r="AL66" s="17"/>
+      <c r="AM66" s="17"/>
+      <c r="AN66" s="17"/>
+      <c r="AO66" s="17"/>
+      <c r="AP66" s="17"/>
+      <c r="AQ66" s="17"/>
+      <c r="AR66" s="17"/>
+      <c r="AS66" s="17"/>
+      <c r="AT66" s="17"/>
+      <c r="AU66" s="17"/>
+      <c r="AV66" s="17"/>
+      <c r="AW66" s="17"/>
+      <c r="AX66" s="17"/>
+      <c r="AY66" s="17"/>
+      <c r="AZ66" s="17"/>
+      <c r="BA66" s="17"/>
+      <c r="BB66" s="17"/>
+      <c r="BC66" s="17"/>
+      <c r="BD66" s="17"/>
+      <c r="BE66" s="17"/>
+      <c r="BF66" s="17"/>
+      <c r="BG66" s="17"/>
+      <c r="BH66" s="17"/>
+      <c r="BI66" s="17"/>
+      <c r="BJ66" s="17"/>
+      <c r="BK66" s="17"/>
+      <c r="BL66" s="17"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="B67" s="16" t="n">
+      <c r="B67" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="15"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
       <c r="I67" s="18"/>
-      <c r="J67" s="22" t="str">
+      <c r="J67" s="19" t="str">
         <f aca="false">IFERROR( ROUNDUP(B67*$Q$80/I67,0), "" )</f>
         <v/>
       </c>
@@ -6330,7 +6204,7 @@
         <f aca="false">IF(I67&gt;0,I67*J67,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L67" s="19"/>
+      <c r="L67" s="21"/>
       <c r="M67" s="20" t="n">
         <f aca="false">L67*$L$77</f>
         <v>0</v>
@@ -6344,76 +6218,76 @@
         <f aca="false">O67*$L$77</f>
         <v>0</v>
       </c>
-      <c r="Q67" s="16"/>
-      <c r="R67" s="16"/>
-      <c r="S67" s="16"/>
-      <c r="T67" s="22"/>
-      <c r="U67" s="16"/>
-      <c r="V67" s="16"/>
-      <c r="W67" s="16"/>
-      <c r="X67" s="16"/>
-      <c r="Y67" s="16"/>
-      <c r="Z67" s="16"/>
-      <c r="AA67" s="16"/>
-      <c r="AB67" s="16"/>
-      <c r="AC67" s="16"/>
-      <c r="AD67" s="16"/>
-      <c r="AE67" s="16"/>
-      <c r="AF67" s="16"/>
-      <c r="AG67" s="16"/>
-      <c r="AH67" s="16"/>
-      <c r="AI67" s="16"/>
-      <c r="AJ67" s="16"/>
-      <c r="AK67" s="16"/>
-      <c r="AL67" s="16"/>
-      <c r="AM67" s="16"/>
-      <c r="AN67" s="16"/>
-      <c r="AO67" s="16"/>
-      <c r="AP67" s="16"/>
-      <c r="AQ67" s="16"/>
-      <c r="AR67" s="16"/>
-      <c r="AS67" s="16"/>
-      <c r="AT67" s="16"/>
-      <c r="AU67" s="16"/>
-      <c r="AV67" s="16"/>
-      <c r="AW67" s="16"/>
-      <c r="AX67" s="16"/>
-      <c r="AY67" s="16"/>
-      <c r="AZ67" s="16"/>
-      <c r="BA67" s="16"/>
-      <c r="BB67" s="16"/>
-      <c r="BC67" s="16"/>
-      <c r="BD67" s="16"/>
-      <c r="BE67" s="16"/>
-      <c r="BF67" s="16"/>
-      <c r="BG67" s="16"/>
-      <c r="BH67" s="16"/>
-      <c r="BI67" s="16"/>
-      <c r="BJ67" s="16"/>
-      <c r="BK67" s="16"/>
-      <c r="BL67" s="16"/>
+      <c r="Q67" s="17"/>
+      <c r="R67" s="17"/>
+      <c r="S67" s="17"/>
+      <c r="T67" s="19"/>
+      <c r="U67" s="17"/>
+      <c r="V67" s="17"/>
+      <c r="W67" s="17"/>
+      <c r="X67" s="17"/>
+      <c r="Y67" s="17"/>
+      <c r="Z67" s="17"/>
+      <c r="AA67" s="17"/>
+      <c r="AB67" s="17"/>
+      <c r="AC67" s="17"/>
+      <c r="AD67" s="17"/>
+      <c r="AE67" s="17"/>
+      <c r="AF67" s="17"/>
+      <c r="AG67" s="17"/>
+      <c r="AH67" s="17"/>
+      <c r="AI67" s="17"/>
+      <c r="AJ67" s="17"/>
+      <c r="AK67" s="17"/>
+      <c r="AL67" s="17"/>
+      <c r="AM67" s="17"/>
+      <c r="AN67" s="17"/>
+      <c r="AO67" s="17"/>
+      <c r="AP67" s="17"/>
+      <c r="AQ67" s="17"/>
+      <c r="AR67" s="17"/>
+      <c r="AS67" s="17"/>
+      <c r="AT67" s="17"/>
+      <c r="AU67" s="17"/>
+      <c r="AV67" s="17"/>
+      <c r="AW67" s="17"/>
+      <c r="AX67" s="17"/>
+      <c r="AY67" s="17"/>
+      <c r="AZ67" s="17"/>
+      <c r="BA67" s="17"/>
+      <c r="BB67" s="17"/>
+      <c r="BC67" s="17"/>
+      <c r="BD67" s="17"/>
+      <c r="BE67" s="17"/>
+      <c r="BF67" s="17"/>
+      <c r="BG67" s="17"/>
+      <c r="BH67" s="17"/>
+      <c r="BI67" s="17"/>
+      <c r="BJ67" s="17"/>
+      <c r="BK67" s="17"/>
+      <c r="BL67" s="17"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="17" t="s">
         <v>344</v>
       </c>
-      <c r="B68" s="16" t="n">
+      <c r="B68" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="15"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16" t="s">
+      <c r="D68" s="17"/>
+      <c r="E68" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="F68" s="16" t="s">
+      <c r="F68" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
       <c r="I68" s="18" t="n">
         <v>600</v>
       </c>
-      <c r="J68" s="22" t="n">
+      <c r="J68" s="19" t="n">
         <f aca="false">IFERROR( ROUNDUP(B68*$Q$80/I68,0), "" )</f>
         <v>1</v>
       </c>
@@ -6421,7 +6295,7 @@
         <f aca="false">IF(I68&gt;0,I68*J68,$Q$80)</f>
         <v>600</v>
       </c>
-      <c r="L68" s="19" t="n">
+      <c r="L68" s="21" t="n">
         <v>5</v>
       </c>
       <c r="M68" s="20" t="n">
@@ -6437,70 +6311,70 @@
         <f aca="false">O68*$L$77</f>
         <v>420</v>
       </c>
-      <c r="Q68" s="16"/>
-      <c r="R68" s="16"/>
-      <c r="S68" s="16"/>
-      <c r="T68" s="22"/>
-      <c r="U68" s="16"/>
-      <c r="V68" s="16"/>
-      <c r="W68" s="16"/>
-      <c r="X68" s="16"/>
-      <c r="Y68" s="16"/>
-      <c r="Z68" s="16"/>
-      <c r="AA68" s="16"/>
-      <c r="AB68" s="16"/>
-      <c r="AC68" s="16"/>
-      <c r="AD68" s="16"/>
-      <c r="AE68" s="16"/>
-      <c r="AF68" s="16"/>
-      <c r="AG68" s="16"/>
-      <c r="AH68" s="16"/>
-      <c r="AI68" s="16"/>
-      <c r="AJ68" s="16"/>
-      <c r="AK68" s="16"/>
-      <c r="AL68" s="16"/>
-      <c r="AM68" s="16"/>
-      <c r="AN68" s="16"/>
-      <c r="AO68" s="16"/>
-      <c r="AP68" s="16"/>
-      <c r="AQ68" s="16"/>
-      <c r="AR68" s="16"/>
-      <c r="AS68" s="16"/>
-      <c r="AT68" s="16"/>
-      <c r="AU68" s="16"/>
-      <c r="AV68" s="16"/>
-      <c r="AW68" s="16"/>
-      <c r="AX68" s="16"/>
-      <c r="AY68" s="16"/>
-      <c r="AZ68" s="16"/>
-      <c r="BA68" s="16"/>
-      <c r="BB68" s="16"/>
-      <c r="BC68" s="16"/>
-      <c r="BD68" s="16"/>
-      <c r="BE68" s="16"/>
-      <c r="BF68" s="16"/>
-      <c r="BG68" s="16"/>
-      <c r="BH68" s="16"/>
-      <c r="BI68" s="16"/>
-      <c r="BJ68" s="16"/>
-      <c r="BK68" s="16"/>
-      <c r="BL68" s="16"/>
+      <c r="Q68" s="17"/>
+      <c r="R68" s="17"/>
+      <c r="S68" s="17"/>
+      <c r="T68" s="19"/>
+      <c r="U68" s="17"/>
+      <c r="V68" s="17"/>
+      <c r="W68" s="17"/>
+      <c r="X68" s="17"/>
+      <c r="Y68" s="17"/>
+      <c r="Z68" s="17"/>
+      <c r="AA68" s="17"/>
+      <c r="AB68" s="17"/>
+      <c r="AC68" s="17"/>
+      <c r="AD68" s="17"/>
+      <c r="AE68" s="17"/>
+      <c r="AF68" s="17"/>
+      <c r="AG68" s="17"/>
+      <c r="AH68" s="17"/>
+      <c r="AI68" s="17"/>
+      <c r="AJ68" s="17"/>
+      <c r="AK68" s="17"/>
+      <c r="AL68" s="17"/>
+      <c r="AM68" s="17"/>
+      <c r="AN68" s="17"/>
+      <c r="AO68" s="17"/>
+      <c r="AP68" s="17"/>
+      <c r="AQ68" s="17"/>
+      <c r="AR68" s="17"/>
+      <c r="AS68" s="17"/>
+      <c r="AT68" s="17"/>
+      <c r="AU68" s="17"/>
+      <c r="AV68" s="17"/>
+      <c r="AW68" s="17"/>
+      <c r="AX68" s="17"/>
+      <c r="AY68" s="17"/>
+      <c r="AZ68" s="17"/>
+      <c r="BA68" s="17"/>
+      <c r="BB68" s="17"/>
+      <c r="BC68" s="17"/>
+      <c r="BD68" s="17"/>
+      <c r="BE68" s="17"/>
+      <c r="BF68" s="17"/>
+      <c r="BG68" s="17"/>
+      <c r="BH68" s="17"/>
+      <c r="BI68" s="17"/>
+      <c r="BJ68" s="17"/>
+      <c r="BK68" s="17"/>
+      <c r="BL68" s="17"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="B69" s="16" t="n">
+      <c r="B69" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="15"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
       <c r="I69" s="18"/>
-      <c r="J69" s="22" t="str">
+      <c r="J69" s="19" t="str">
         <f aca="false">IFERROR( ROUNDUP(B69*$Q$80/I69,0), "" )</f>
         <v/>
       </c>
@@ -6508,7 +6382,7 @@
         <f aca="false">IF(I69&gt;0,I69*J69,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L69" s="19" t="n">
+      <c r="L69" s="21" t="n">
         <v>22</v>
       </c>
       <c r="M69" s="20" t="n">
@@ -6524,70 +6398,70 @@
         <f aca="false">O69*$L$77</f>
         <v>1694</v>
       </c>
-      <c r="Q69" s="16"/>
-      <c r="R69" s="16"/>
+      <c r="Q69" s="17"/>
+      <c r="R69" s="17"/>
       <c r="S69" s="15"/>
-      <c r="T69" s="16"/>
-      <c r="U69" s="22"/>
-      <c r="V69" s="16"/>
-      <c r="W69" s="22"/>
-      <c r="X69" s="22"/>
-      <c r="Y69" s="22"/>
-      <c r="Z69" s="22"/>
-      <c r="AA69" s="22"/>
-      <c r="AB69" s="22"/>
-      <c r="AC69" s="22"/>
-      <c r="AD69" s="22"/>
-      <c r="AE69" s="22"/>
-      <c r="AF69" s="22"/>
-      <c r="AG69" s="22"/>
-      <c r="AH69" s="22"/>
-      <c r="AI69" s="22"/>
-      <c r="AJ69" s="22"/>
-      <c r="AK69" s="22"/>
-      <c r="AL69" s="22"/>
-      <c r="AM69" s="22"/>
-      <c r="AN69" s="22"/>
-      <c r="AO69" s="22"/>
-      <c r="AP69" s="22"/>
-      <c r="AQ69" s="22"/>
-      <c r="AR69" s="22"/>
-      <c r="AS69" s="22"/>
-      <c r="AT69" s="22"/>
-      <c r="AU69" s="22"/>
-      <c r="AV69" s="22"/>
-      <c r="AW69" s="22"/>
-      <c r="AX69" s="22"/>
-      <c r="AY69" s="22"/>
-      <c r="AZ69" s="22"/>
-      <c r="BA69" s="22"/>
-      <c r="BB69" s="22"/>
-      <c r="BC69" s="22"/>
-      <c r="BD69" s="22"/>
-      <c r="BE69" s="22"/>
-      <c r="BF69" s="22"/>
-      <c r="BG69" s="22"/>
-      <c r="BH69" s="22"/>
-      <c r="BI69" s="22"/>
-      <c r="BJ69" s="22"/>
-      <c r="BK69" s="22"/>
-      <c r="BL69" s="22"/>
+      <c r="T69" s="17"/>
+      <c r="U69" s="19"/>
+      <c r="V69" s="17"/>
+      <c r="W69" s="19"/>
+      <c r="X69" s="19"/>
+      <c r="Y69" s="19"/>
+      <c r="Z69" s="19"/>
+      <c r="AA69" s="19"/>
+      <c r="AB69" s="19"/>
+      <c r="AC69" s="19"/>
+      <c r="AD69" s="19"/>
+      <c r="AE69" s="19"/>
+      <c r="AF69" s="19"/>
+      <c r="AG69" s="19"/>
+      <c r="AH69" s="19"/>
+      <c r="AI69" s="19"/>
+      <c r="AJ69" s="19"/>
+      <c r="AK69" s="19"/>
+      <c r="AL69" s="19"/>
+      <c r="AM69" s="19"/>
+      <c r="AN69" s="19"/>
+      <c r="AO69" s="19"/>
+      <c r="AP69" s="19"/>
+      <c r="AQ69" s="19"/>
+      <c r="AR69" s="19"/>
+      <c r="AS69" s="19"/>
+      <c r="AT69" s="19"/>
+      <c r="AU69" s="19"/>
+      <c r="AV69" s="19"/>
+      <c r="AW69" s="19"/>
+      <c r="AX69" s="19"/>
+      <c r="AY69" s="19"/>
+      <c r="AZ69" s="19"/>
+      <c r="BA69" s="19"/>
+      <c r="BB69" s="19"/>
+      <c r="BC69" s="19"/>
+      <c r="BD69" s="19"/>
+      <c r="BE69" s="19"/>
+      <c r="BF69" s="19"/>
+      <c r="BG69" s="19"/>
+      <c r="BH69" s="19"/>
+      <c r="BI69" s="19"/>
+      <c r="BJ69" s="19"/>
+      <c r="BK69" s="19"/>
+      <c r="BL69" s="19"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="B70" s="16" t="n">
+      <c r="B70" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="15"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
       <c r="I70" s="18"/>
-      <c r="J70" s="22" t="str">
+      <c r="J70" s="19" t="str">
         <f aca="false">IFERROR( ROUNDUP(B70*$Q$80/I70,0), "" )</f>
         <v/>
       </c>
@@ -6595,7 +6469,7 @@
         <f aca="false">IF(I70&gt;0,I70*J70,$Q$80)</f>
         <v>550</v>
       </c>
-      <c r="L70" s="19" t="n">
+      <c r="L70" s="21" t="n">
         <v>25</v>
       </c>
       <c r="M70" s="20" t="n">
@@ -6611,54 +6485,54 @@
         <f aca="false">O70*$L$77</f>
         <v>1925</v>
       </c>
-      <c r="Q70" s="16"/>
-      <c r="R70" s="16"/>
+      <c r="Q70" s="17"/>
+      <c r="R70" s="17"/>
       <c r="S70" s="15"/>
-      <c r="T70" s="16"/>
-      <c r="U70" s="22"/>
-      <c r="V70" s="16"/>
-      <c r="W70" s="22"/>
-      <c r="X70" s="22"/>
-      <c r="Y70" s="22"/>
-      <c r="Z70" s="22"/>
-      <c r="AA70" s="22"/>
-      <c r="AB70" s="22"/>
-      <c r="AC70" s="22"/>
-      <c r="AD70" s="22"/>
-      <c r="AE70" s="22"/>
-      <c r="AF70" s="22"/>
-      <c r="AG70" s="22"/>
-      <c r="AH70" s="22"/>
-      <c r="AI70" s="22"/>
-      <c r="AJ70" s="22"/>
-      <c r="AK70" s="22"/>
-      <c r="AL70" s="22"/>
-      <c r="AM70" s="22"/>
-      <c r="AN70" s="22"/>
-      <c r="AO70" s="22"/>
-      <c r="AP70" s="22"/>
-      <c r="AQ70" s="22"/>
-      <c r="AR70" s="22"/>
-      <c r="AS70" s="22"/>
-      <c r="AT70" s="22"/>
-      <c r="AU70" s="22"/>
-      <c r="AV70" s="22"/>
-      <c r="AW70" s="22"/>
-      <c r="AX70" s="22"/>
-      <c r="AY70" s="22"/>
-      <c r="AZ70" s="22"/>
-      <c r="BA70" s="22"/>
-      <c r="BB70" s="22"/>
-      <c r="BC70" s="22"/>
-      <c r="BD70" s="22"/>
-      <c r="BE70" s="22"/>
-      <c r="BF70" s="22"/>
-      <c r="BG70" s="22"/>
-      <c r="BH70" s="22"/>
-      <c r="BI70" s="22"/>
-      <c r="BJ70" s="22"/>
-      <c r="BK70" s="22"/>
-      <c r="BL70" s="22"/>
+      <c r="T70" s="17"/>
+      <c r="U70" s="19"/>
+      <c r="V70" s="17"/>
+      <c r="W70" s="19"/>
+      <c r="X70" s="19"/>
+      <c r="Y70" s="19"/>
+      <c r="Z70" s="19"/>
+      <c r="AA70" s="19"/>
+      <c r="AB70" s="19"/>
+      <c r="AC70" s="19"/>
+      <c r="AD70" s="19"/>
+      <c r="AE70" s="19"/>
+      <c r="AF70" s="19"/>
+      <c r="AG70" s="19"/>
+      <c r="AH70" s="19"/>
+      <c r="AI70" s="19"/>
+      <c r="AJ70" s="19"/>
+      <c r="AK70" s="19"/>
+      <c r="AL70" s="19"/>
+      <c r="AM70" s="19"/>
+      <c r="AN70" s="19"/>
+      <c r="AO70" s="19"/>
+      <c r="AP70" s="19"/>
+      <c r="AQ70" s="19"/>
+      <c r="AR70" s="19"/>
+      <c r="AS70" s="19"/>
+      <c r="AT70" s="19"/>
+      <c r="AU70" s="19"/>
+      <c r="AV70" s="19"/>
+      <c r="AW70" s="19"/>
+      <c r="AX70" s="19"/>
+      <c r="AY70" s="19"/>
+      <c r="AZ70" s="19"/>
+      <c r="BA70" s="19"/>
+      <c r="BB70" s="19"/>
+      <c r="BC70" s="19"/>
+      <c r="BD70" s="19"/>
+      <c r="BE70" s="19"/>
+      <c r="BF70" s="19"/>
+      <c r="BG70" s="19"/>
+      <c r="BH70" s="19"/>
+      <c r="BI70" s="19"/>
+      <c r="BJ70" s="19"/>
+      <c r="BK70" s="19"/>
+      <c r="BL70" s="19"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I73" s="8"/>
@@ -6673,7 +6547,7 @@
         <f aca="false">SUM(O2:O72)</f>
         <v>111540.24</v>
       </c>
-      <c r="P73" s="8" t="n">
+      <c r="P73" s="22" t="n">
         <f aca="false">SUM(P2:P72)</f>
         <v>15615.6336</v>
       </c>

</xml_diff>